<commit_message>
more graph and auc
</commit_message>
<xml_diff>
--- a/output/class1_stat_report.xlsx
+++ b/output/class1_stat_report.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="20">
   <si>
     <t>selectivity</t>
   </si>
@@ -25,16 +25,55 @@
     <t>accuracy</t>
   </si>
   <si>
-    <t>0.96</t>
+    <t>0.92</t>
+  </si>
+  <si>
+    <t>0.75</t>
+  </si>
+  <si>
+    <t>0.83</t>
+  </si>
+  <si>
+    <t>0.76</t>
   </si>
   <si>
     <t>1.00</t>
   </si>
   <si>
-    <t>0.98</t>
-  </si>
-  <si>
-    <t>0.92</t>
+    <t>0.86</t>
+  </si>
+  <si>
+    <t>0.84</t>
+  </si>
+  <si>
+    <t>0.91</t>
+  </si>
+  <si>
+    <t>0.80</t>
+  </si>
+  <si>
+    <t>0.89</t>
+  </si>
+  <si>
+    <t>0.94</t>
+  </si>
+  <si>
+    <t>0.97</t>
+  </si>
+  <si>
+    <t>0.88</t>
+  </si>
+  <si>
+    <t>0.93</t>
+  </si>
+  <si>
+    <t>0.90</t>
+  </si>
+  <si>
+    <t>0.81</t>
+  </si>
+  <si>
+    <t>0.87</t>
   </si>
 </sst>
 </file>
@@ -396,57 +435,57 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="B6" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C6" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="B7" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="C7" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -454,40 +493,40 @@
         <v>4</v>
       </c>
       <c r="B8" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="C8" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="B9" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="C9" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="B10" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="C10" t="s">
-        <v>3</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11" t="s">
         <v>4</v>
-      </c>
-      <c r="B11" t="s">
-        <v>3</v>
       </c>
       <c r="C11" t="s">
         <v>5</v>

</xml_diff>